<commit_message>
make new figures and improve script
</commit_message>
<xml_diff>
--- a/simulation_results_glmm/April10_fullsimulation/summary-results-bias-g10-edit.xlsx
+++ b/simulation_results_glmm/April10_fullsimulation/summary-results-bias-g10-edit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\warde\Documents\GitHub\Master-Thesis\simulation_results_glmm\April10_fullsimulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A351FECF-FAA3-4D4E-8080-D88800CEF9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AA43CD-4743-4F39-93F2-ACD3D72007A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4AB77A2F-E666-4F15-A688-EF80F5E9D49A}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4AB77A2F-E666-4F15-A688-EF80F5E9D49A}"/>
   </bookViews>
   <sheets>
     <sheet name="summary-results-bias-g10" sheetId="1" r:id="rId1"/>
@@ -685,6 +685,11 @@
         <filter val="binary"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{F4BA8D42-524B-4290-B826-DC56FAAD07D6}" name="N_total"/>
@@ -1051,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAAF8D1-3696-476D-8F94-1162B3C50468}">
   <dimension ref="A1:AN379"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H362" sqref="H362:H367"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O115" sqref="O115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1216,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1333,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -1455,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -1577,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>200</v>
       </c>
@@ -1699,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -1821,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>200</v>
       </c>
@@ -3407,7 +3412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>100</v>
       </c>
@@ -3529,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>200</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -3773,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>200</v>
       </c>
@@ -3895,7 +3900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>100</v>
       </c>
@@ -4017,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>200</v>
       </c>
@@ -7799,7 +7804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>100</v>
       </c>
@@ -7921,7 +7926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>200</v>
       </c>
@@ -8043,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>100</v>
       </c>
@@ -8165,7 +8170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>200</v>
       </c>
@@ -8287,7 +8292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>100</v>
       </c>
@@ -8409,7 +8414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>200</v>
       </c>
@@ -12191,7 +12196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>100</v>
       </c>
@@ -12313,7 +12318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>200</v>
       </c>
@@ -12435,7 +12440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>100</v>
       </c>
@@ -12557,7 +12562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>200</v>
       </c>
@@ -12679,7 +12684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>100</v>
       </c>
@@ -12801,7 +12806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>200</v>
       </c>
@@ -16583,7 +16588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>100</v>
       </c>
@@ -16705,7 +16710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>200</v>
       </c>
@@ -16827,7 +16832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>100</v>
       </c>
@@ -16949,7 +16954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>200</v>
       </c>
@@ -17071,7 +17076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>100</v>
       </c>
@@ -17193,7 +17198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>200</v>
       </c>
@@ -18779,7 +18784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>100</v>
       </c>
@@ -18901,7 +18906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>200</v>
       </c>
@@ -19023,7 +19028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>100</v>
       </c>
@@ -19145,7 +19150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>200</v>
       </c>
@@ -19267,7 +19272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>100</v>
       </c>
@@ -19389,7 +19394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>200</v>
       </c>
@@ -23171,7 +23176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>100</v>
       </c>
@@ -23293,7 +23298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>200</v>
       </c>
@@ -23415,7 +23420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>100</v>
       </c>
@@ -23537,7 +23542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>200</v>
       </c>
@@ -23659,7 +23664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>100</v>
       </c>
@@ -23781,7 +23786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>200</v>
       </c>
@@ -27563,7 +27568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>100</v>
       </c>
@@ -27685,7 +27690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>200</v>
       </c>
@@ -27807,7 +27812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>100</v>
       </c>
@@ -27929,7 +27934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>200</v>
       </c>
@@ -28051,7 +28056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>100</v>
       </c>
@@ -28173,7 +28178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>200</v>
       </c>
@@ -31955,7 +31960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>100</v>
       </c>
@@ -32077,7 +32082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>200</v>
       </c>
@@ -32199,7 +32204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>100</v>
       </c>
@@ -32321,7 +32326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>200</v>
       </c>
@@ -32443,7 +32448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>100</v>
       </c>
@@ -32565,7 +32570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>200</v>
       </c>
@@ -34151,7 +34156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>100</v>
       </c>
@@ -34273,7 +34278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>200</v>
       </c>
@@ -34395,7 +34400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>100</v>
       </c>
@@ -34517,7 +34522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>200</v>
       </c>
@@ -34639,7 +34644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>100</v>
       </c>
@@ -34761,7 +34766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>200</v>
       </c>
@@ -38543,7 +38548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>100</v>
       </c>
@@ -38665,7 +38670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>200</v>
       </c>
@@ -38787,7 +38792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>100</v>
       </c>
@@ -38909,7 +38914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>200</v>
       </c>
@@ -39031,7 +39036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>100</v>
       </c>
@@ -39153,7 +39158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>200</v>
       </c>
@@ -42935,7 +42940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>100</v>
       </c>
@@ -43057,7 +43062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>200</v>
       </c>
@@ -43179,7 +43184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>100</v>
       </c>
@@ -43301,7 +43306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>200</v>
       </c>
@@ -43423,7 +43428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>100</v>
       </c>
@@ -43545,7 +43550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>200</v>
       </c>

</xml_diff>